<commit_message>
rerunning everything with updated dds design
</commit_message>
<xml_diff>
--- a/gene_expression/sample_metadata.xlsx
+++ b/gene_expression/sample_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch4_AcerCCC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch4_AcerCCC/gene_expression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C2B134F0-D627-3740-8162-372010AFAF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07235F8F-3553-1244-82D7-D7F91B73DCBC}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{C2B134F0-D627-3740-8162-372010AFAF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A85E921-96A0-8C45-B263-A83A14625FBC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{64624594-119B-0044-8A32-F7F4760EE2EE}"/>
   </bookViews>
@@ -130,6 +130,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,7 +456,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,13 +486,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -499,13 +503,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -516,13 +520,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>1099</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -533,13 +537,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -550,13 +554,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>1087</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -567,13 +571,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>1089</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -584,13 +588,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -601,13 +605,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1096</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -621,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>1090</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -635,13 +639,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -720,13 +724,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>2382</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -737,13 +741,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1">
-        <v>2383</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -754,13 +758,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
       </c>
       <c r="E18" s="1">
-        <v>2384</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -771,13 +775,13 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>2266</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -788,13 +792,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>2267</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -805,19 +809,18 @@
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>2268</v>
+        <v>2384</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
-    <sortCondition ref="A2:A21"/>
-    <sortCondition ref="C2:C21"/>
+    <sortCondition ref="E2:E21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>